<commit_message>
Update testing on live application.xlsx
</commit_message>
<xml_diff>
--- a/Assingment/testing on live application.xlsx
+++ b/Assingment/testing on live application.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5bcf8b3e57f56cfd/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5bcf8b3e57f56cfd/Documents/GitHub/Karan-Testing/Assingment/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="133" documentId="8_{9DE17FFA-F617-4E1C-BFFD-53F9C9E8C81A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A3384A7B-5C87-47F4-A798-9CF6FAA14FA0}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{1021690B-F835-467C-AED6-E1B1B6295AAE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1021690B-F835-467C-AED6-E1B1B6295AAE}"/>
   </bookViews>
   <sheets>
     <sheet name="HLR" sheetId="2" r:id="rId1"/>
@@ -888,6 +888,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -909,9 +912,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -927,10 +927,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1232,7 +1228,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E93CA792-1B87-49D1-8988-1CAF30E9F11B}">
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
@@ -1244,11 +1240,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
     </row>
     <row r="2" spans="1:3" ht="42" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -1514,7 +1510,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>301</v>
       </c>
@@ -1525,7 +1521,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>302</v>
       </c>
@@ -1581,10 +1577,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="11"/>
+      <c r="B1" s="12"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1743,16 +1739,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="14"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="15"/>
     </row>
     <row r="2" spans="1:8" ht="36" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
@@ -1781,782 +1777,782 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="16">
+      <c r="A3" s="9">
         <v>1</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="C3" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="D3" s="16" t="s">
+      <c r="C3" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="E3" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="F3" s="16" t="s">
+      <c r="E3" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F3" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="G3" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="H3" s="16" t="s">
+      <c r="G3" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="H3" s="9" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="72" x14ac:dyDescent="0.3">
-      <c r="A4" s="16">
+      <c r="A4" s="9">
         <v>2</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="C4" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="D4" s="16" t="s">
+      <c r="C4" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="E4" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="F4" s="16" t="s">
+      <c r="E4" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F4" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="G4" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="H4" s="16" t="s">
+      <c r="G4" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="H4" s="9" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A5" s="16">
+      <c r="A5" s="9">
         <v>2</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="C5" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="D5" s="16" t="s">
+      <c r="C5" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D5" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="E5" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="F5" s="16" t="s">
+      <c r="E5" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F5" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="G5" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="H5" s="16" t="s">
+      <c r="G5" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="H5" s="9" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A6" s="16">
+      <c r="A6" s="9">
         <v>2</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="C6" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="D6" s="16" t="s">
+      <c r="C6" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="E6" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="F6" s="16" t="s">
+      <c r="E6" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F6" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="G6" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="H6" s="16" t="s">
+      <c r="G6" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="H6" s="9" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A7" s="16">
+      <c r="A7" s="9">
         <v>2</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="C7" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="D7" s="16" t="s">
+      <c r="C7" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="E7" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="F7" s="16" t="s">
+      <c r="E7" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F7" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="G7" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="H7" s="16" t="s">
+      <c r="G7" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="H7" s="9" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A8" s="16">
+      <c r="A8" s="9">
         <v>2</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="C8" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="D8" s="16" t="s">
+      <c r="C8" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="E8" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="F8" s="16" t="s">
+      <c r="E8" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F8" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="G8" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="H8" s="16" t="s">
+      <c r="G8" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="H8" s="9" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A9" s="16">
+      <c r="A9" s="9">
         <v>2</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="C9" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="D9" s="16" t="s">
+      <c r="C9" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D9" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="E9" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="F9" s="16" t="s">
+      <c r="E9" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F9" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="G9" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="H9" s="16" t="s">
+      <c r="G9" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="H9" s="9" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A10" s="16">
+      <c r="A10" s="9">
         <v>2</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="C10" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="D10" s="16" t="s">
+      <c r="C10" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="E10" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="F10" s="16" t="s">
+      <c r="E10" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F10" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="G10" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="H10" s="16" t="s">
+      <c r="G10" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="H10" s="9" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A11" s="16">
+      <c r="A11" s="9">
         <v>2</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="C11" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="D11" s="16" t="s">
+      <c r="C11" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="E11" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="F11" s="16" t="s">
+      <c r="E11" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F11" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="G11" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="H11" s="16" t="s">
+      <c r="G11" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="H11" s="9" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A12" s="16">
+      <c r="A12" s="9">
         <v>2</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="C12" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="D12" s="16" t="s">
+      <c r="C12" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="E12" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="F12" s="16" t="s">
+      <c r="E12" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F12" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="G12" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="H12" s="16" t="s">
+      <c r="G12" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="H12" s="9" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="72" x14ac:dyDescent="0.3">
-      <c r="A13" s="16">
+      <c r="A13" s="9">
         <v>3</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="C13" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="D13" s="16" t="s">
+      <c r="C13" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D13" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="E13" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="F13" s="16" t="s">
+      <c r="E13" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F13" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="G13" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="H13" s="16" t="s">
+      <c r="G13" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="H13" s="9" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A14" s="16">
+      <c r="A14" s="9">
         <v>3</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="C14" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="D14" s="16" t="s">
+      <c r="C14" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D14" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="E14" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="F14" s="16" t="s">
+      <c r="E14" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F14" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="G14" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="H14" s="16" t="s">
+      <c r="G14" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="H14" s="9" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A15" s="16">
+      <c r="A15" s="9">
         <v>3</v>
       </c>
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="C15" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="D15" s="16" t="s">
+      <c r="C15" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D15" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="E15" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="F15" s="16" t="s">
+      <c r="E15" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F15" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="G15" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="H15" s="16" t="s">
+      <c r="G15" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="H15" s="9" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="72" x14ac:dyDescent="0.3">
-      <c r="A16" s="16">
+      <c r="A16" s="9">
         <v>4</v>
       </c>
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="C16" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="D16" s="16" t="s">
+      <c r="C16" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D16" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="E16" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="F16" s="16" t="s">
+      <c r="E16" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F16" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="G16" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="H16" s="16" t="s">
+      <c r="G16" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="H16" s="9" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A17" s="16">
+      <c r="A17" s="9">
         <v>4</v>
       </c>
-      <c r="B17" s="16" t="s">
+      <c r="B17" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="C17" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="D17" s="16" t="s">
+      <c r="C17" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="E17" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="F17" s="16" t="s">
+      <c r="E17" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F17" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="G17" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="H17" s="16" t="s">
+      <c r="G17" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="H17" s="9" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A18" s="16">
+      <c r="A18" s="9">
         <v>4</v>
       </c>
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="C18" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="D18" s="16" t="s">
+      <c r="C18" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D18" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="E18" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="F18" s="16" t="s">
+      <c r="E18" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F18" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="G18" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="H18" s="16" t="s">
+      <c r="G18" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="H18" s="9" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A19" s="16">
+      <c r="A19" s="9">
         <v>4</v>
       </c>
-      <c r="B19" s="16" t="s">
+      <c r="B19" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="C19" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="D19" s="16" t="s">
+      <c r="C19" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D19" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="E19" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="F19" s="16" t="s">
+      <c r="E19" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F19" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="G19" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="H19" s="16" t="s">
+      <c r="G19" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="H19" s="9" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A20" s="16">
+      <c r="A20" s="9">
         <v>4</v>
       </c>
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="C20" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="D20" s="16" t="s">
+      <c r="C20" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D20" s="9" t="s">
         <v>176</v>
       </c>
-      <c r="E20" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="F20" s="16" t="s">
+      <c r="E20" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F20" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="G20" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="H20" s="16" t="s">
+      <c r="G20" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="H20" s="9" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A21" s="16">
+      <c r="A21" s="9">
         <v>4</v>
       </c>
-      <c r="B21" s="16" t="s">
+      <c r="B21" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="C21" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="D21" s="16" t="s">
+      <c r="C21" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D21" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="E21" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="F21" s="16" t="s">
+      <c r="E21" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F21" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="G21" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="H21" s="16" t="s">
+      <c r="G21" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="H21" s="9" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A22" s="16">
+      <c r="A22" s="9">
         <v>4</v>
       </c>
-      <c r="B22" s="16" t="s">
+      <c r="B22" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="C22" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="D22" s="16" t="s">
+      <c r="C22" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D22" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="E22" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="F22" s="16" t="s">
+      <c r="E22" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F22" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="G22" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="H22" s="16" t="s">
+      <c r="G22" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="H22" s="9" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A23" s="16">
+      <c r="A23" s="9">
         <v>4</v>
       </c>
-      <c r="B23" s="16" t="s">
+      <c r="B23" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="C23" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="D23" s="16" t="s">
+      <c r="C23" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D23" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="E23" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="F23" s="16" t="s">
+      <c r="E23" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F23" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="G23" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="H23" s="16" t="s">
+      <c r="G23" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="H23" s="9" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="72" x14ac:dyDescent="0.3">
-      <c r="A24" s="16">
+      <c r="A24" s="9">
         <v>5</v>
       </c>
-      <c r="B24" s="16" t="s">
+      <c r="B24" s="9" t="s">
         <v>184</v>
       </c>
-      <c r="C24" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="D24" s="16" t="s">
+      <c r="C24" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D24" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="E24" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="F24" s="16" t="s">
+      <c r="E24" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F24" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="G24" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="H24" s="16" t="s">
+      <c r="G24" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="H24" s="9" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A25" s="16">
+      <c r="A25" s="9">
         <v>5</v>
       </c>
-      <c r="B25" s="16" t="s">
+      <c r="B25" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="C25" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="D25" s="16" t="s">
+      <c r="C25" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D25" s="9" t="s">
         <v>187</v>
       </c>
-      <c r="E25" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="F25" s="16" t="s">
+      <c r="E25" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F25" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="G25" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="H25" s="16" t="s">
+      <c r="G25" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="H25" s="9" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A26" s="16">
+      <c r="A26" s="9">
         <v>5</v>
       </c>
-      <c r="B26" s="16" t="s">
+      <c r="B26" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="C26" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="D26" s="16" t="s">
+      <c r="C26" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D26" s="9" t="s">
         <v>189</v>
       </c>
-      <c r="E26" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="F26" s="16" t="s">
+      <c r="E26" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F26" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="G26" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="H26" s="16" t="s">
+      <c r="G26" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="H26" s="9" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A27" s="16">
+      <c r="A27" s="9">
         <v>5</v>
       </c>
-      <c r="B27" s="16" t="s">
+      <c r="B27" s="9" t="s">
         <v>191</v>
       </c>
-      <c r="C27" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="D27" s="16" t="s">
+      <c r="C27" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D27" s="9" t="s">
         <v>192</v>
       </c>
-      <c r="E27" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="F27" s="16" t="s">
+      <c r="E27" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F27" s="9" t="s">
         <v>193</v>
       </c>
-      <c r="G27" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="H27" s="16" t="s">
+      <c r="G27" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="H27" s="9" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A28" s="16">
+      <c r="A28" s="9">
         <v>5</v>
       </c>
-      <c r="B28" s="16" t="s">
+      <c r="B28" s="9" t="s">
         <v>194</v>
       </c>
-      <c r="C28" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="D28" s="16" t="s">
+      <c r="C28" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D28" s="9" t="s">
         <v>195</v>
       </c>
-      <c r="E28" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="F28" s="16" t="s">
+      <c r="E28" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F28" s="9" t="s">
         <v>196</v>
       </c>
-      <c r="G28" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="H28" s="16" t="s">
+      <c r="G28" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="H28" s="9" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A29" s="16">
+      <c r="A29" s="9">
         <v>5</v>
       </c>
-      <c r="B29" s="16" t="s">
+      <c r="B29" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="C29" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="D29" s="16" t="s">
+      <c r="C29" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D29" s="9" t="s">
         <v>197</v>
       </c>
-      <c r="E29" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="F29" s="16" t="s">
+      <c r="E29" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F29" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="G29" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="H29" s="16" t="s">
+      <c r="G29" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="H29" s="9" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A30" s="16">
+      <c r="A30" s="9">
         <v>5</v>
       </c>
-      <c r="B30" s="16" t="s">
+      <c r="B30" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="C30" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="D30" s="16" t="s">
+      <c r="C30" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D30" s="9" t="s">
         <v>198</v>
       </c>
-      <c r="E30" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="F30" s="16" t="s">
+      <c r="E30" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F30" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="G30" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="H30" s="16" t="s">
+      <c r="G30" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="H30" s="9" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A31" s="16">
+      <c r="A31" s="9">
         <v>5</v>
       </c>
-      <c r="B31" s="16" t="s">
+      <c r="B31" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="C31" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="D31" s="16" t="s">
+      <c r="C31" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D31" s="9" t="s">
         <v>199</v>
       </c>
-      <c r="E31" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="F31" s="16" t="s">
+      <c r="E31" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F31" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="G31" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="H31" s="16" t="s">
+      <c r="G31" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="H31" s="9" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A32" s="16">
+      <c r="A32" s="9">
         <v>5</v>
       </c>
-      <c r="B32" s="16" t="s">
+      <c r="B32" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="C32" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="D32" s="16" t="s">
+      <c r="C32" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D32" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="E32" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="F32" s="16" t="s">
+      <c r="E32" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F32" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="G32" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="H32" s="16" t="s">
+      <c r="G32" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="H32" s="9" t="s">
         <v>64</v>
       </c>
     </row>
@@ -2573,7 +2569,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0A72C13-7E58-4BB1-AB6C-DF1603EFC30C}">
   <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
@@ -2664,7 +2660,7 @@
       </c>
     </row>
     <row r="11" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="16" t="s">
         <v>147</v>
       </c>
       <c r="B11" s="8" t="s">
@@ -2672,19 +2668,19 @@
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="15"/>
+      <c r="A12" s="16"/>
       <c r="B12" s="8" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="15"/>
+      <c r="A13" s="16"/>
       <c r="B13" s="8" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="15"/>
+      <c r="A14" s="16"/>
       <c r="B14" s="8" t="s">
         <v>149</v>
       </c>
@@ -2722,7 +2718,7 @@
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="15" t="s">
+      <c r="A19" s="16" t="s">
         <v>158</v>
       </c>
       <c r="B19" s="8" t="s">
@@ -2730,25 +2726,25 @@
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="15"/>
+      <c r="A20" s="16"/>
       <c r="B20" s="8" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="15"/>
+      <c r="A21" s="16"/>
       <c r="B21" s="8" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="15"/>
+      <c r="A22" s="16"/>
       <c r="B22" s="8" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="15" t="s">
+      <c r="A23" s="16" t="s">
         <v>159</v>
       </c>
       <c r="B23" s="8" t="s">
@@ -2756,7 +2752,7 @@
       </c>
     </row>
     <row r="24" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A24" s="15"/>
+      <c r="A24" s="16"/>
       <c r="B24" s="8" t="s">
         <v>161</v>
       </c>

</xml_diff>